<commit_message>
Added images and made some minor adjustments to 'Working_Estimator_Script'
</commit_message>
<xml_diff>
--- a/HD_df.xlsx
+++ b/HD_df.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kijah\Documents\Data_Bootcamp\Estimator_Project\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6833504F-5A2C-4320-8BD1-36FD93FCF4C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="38">
   <si>
     <t>Material_Description</t>
   </si>
@@ -125,13 +131,16 @@
   </si>
   <si>
     <t>Home Depot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16 ITEMS WE ARE PRICE TRACKING </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,21 +156,122 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="13">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -171,11 +281,63 @@
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="thin">
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color auto="1"/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -183,17 +345,41 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -240,7 +426,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -272,9 +458,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -306,6 +510,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -481,252 +703,268 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="64.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.73046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.59765625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="21.4" thickBot="1" x14ac:dyDescent="0.7">
+      <c r="A1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="3"/>
+    </row>
+    <row r="2" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="10" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C2">
+      <c r="C3" s="11">
         <v>20.62</v>
       </c>
-      <c r="D2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
+      <c r="D3" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C3">
+      <c r="C4" s="12">
         <v>11.91</v>
       </c>
-      <c r="D3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
+      <c r="D4" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C4">
+      <c r="C5" s="12">
         <v>3.98</v>
       </c>
-      <c r="D4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
+      <c r="D5" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C5">
+      <c r="C6" s="12">
         <v>7.22</v>
       </c>
-      <c r="D5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
+      <c r="D6" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C6">
-        <v>1.15</v>
-      </c>
-      <c r="D6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
+      <c r="C7" s="12">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="C7">
+      <c r="C8" s="12">
         <v>2.34</v>
       </c>
-      <c r="D7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
+      <c r="D8" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C8">
+      <c r="C9" s="12">
         <v>3.68</v>
       </c>
-      <c r="D8" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s">
+      <c r="D9" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C9">
+      <c r="C10" s="12">
         <v>1.28</v>
       </c>
-      <c r="D9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
+      <c r="D10" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A11" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C10">
+      <c r="C11" s="12">
         <v>2.98</v>
       </c>
-      <c r="D10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" t="s">
+      <c r="D11" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A12" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C11">
+      <c r="C12" s="12">
         <v>787</v>
       </c>
-      <c r="D11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" t="s">
+      <c r="D12" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A13" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C12">
+      <c r="C13" s="12">
         <v>425</v>
       </c>
-      <c r="D12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" t="s">
+      <c r="D13" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A14" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="C13">
+      <c r="C14" s="12">
         <v>159</v>
       </c>
-      <c r="D13" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" t="s">
+      <c r="D14" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A15" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="C14">
+      <c r="C15" s="12">
         <v>118</v>
       </c>
-      <c r="D14" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" t="s">
+      <c r="D15" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A16" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="C15">
+      <c r="C16" s="12">
         <v>159</v>
       </c>
-      <c r="D15" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" t="s">
+      <c r="D16" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A17" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="C16">
+      <c r="C17" s="12">
         <v>149</v>
       </c>
-      <c r="D16" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" t="s">
+      <c r="D17" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A18" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="C17">
+      <c r="C18" s="13">
         <v>289</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D18" s="7" t="s">
         <v>36</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="B3:B18" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>